<commit_message>
dobavjane na izkljucenija. Opravjane na drebni problemi
</commit_message>
<xml_diff>
--- a/arhiv/New folder/recnik_za_o.xlsx
+++ b/arhiv/New folder/recnik_za_o.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiko\PycharmProjects\novpisane\arhiv\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B29631-EA12-4814-9256-A157355A5D5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920A6CDA-1FC7-49F7-8877-CACE15EE5A30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3504" uniqueCount="3034">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3504" uniqueCount="3161">
   <si>
     <t>abhorrence</t>
   </si>
@@ -9122,6 +9122,387 @@
   </si>
   <si>
     <t>RÝʃɒT</t>
+  </si>
+  <si>
+    <t>RÏSɒTÖ</t>
+  </si>
+  <si>
+    <t>RɒS©</t>
+  </si>
+  <si>
+    <t>RɒSIÑ</t>
+  </si>
+  <si>
+    <t>Rɒθ©</t>
+  </si>
+  <si>
+    <t>RɒθS</t>
+  </si>
+  <si>
+    <t>RÚDɒLF/RÚDɒF</t>
+  </si>
+  <si>
+    <t>RʌNɒF</t>
+  </si>
+  <si>
+    <t>SɒNKÚLɒT</t>
+  </si>
+  <si>
+    <t>SɛRəTɒV/SɛRəTɒF</t>
+  </si>
+  <si>
+    <t>S©ɒÑ</t>
+  </si>
+  <si>
+    <t>S©ɒÑZ</t>
+  </si>
+  <si>
+    <t>SKɒF</t>
+  </si>
+  <si>
+    <t>SKɒFђ</t>
+  </si>
+  <si>
+    <t>SKɒFS</t>
+  </si>
+  <si>
+    <t>SNɒT</t>
+  </si>
+  <si>
+    <t>SNɒTFÉS</t>
+  </si>
+  <si>
+    <t>SNɒTFÉSђ</t>
+  </si>
+  <si>
+    <t>SNɒTÏ</t>
+  </si>
+  <si>
+    <t>SɒDəM</t>
+  </si>
+  <si>
+    <t>SɒFIT</t>
+  </si>
+  <si>
+    <t>SɒFTBɔL/SɒFBɔL</t>
+  </si>
+  <si>
+    <t>SɒFTBɔLZ/SɒFBɔLZ</t>
+  </si>
+  <si>
+    <t>SɒFəNћ</t>
+  </si>
+  <si>
+    <t>SɒFəN©</t>
+  </si>
+  <si>
+    <t>SɒFəNIÑ/SɒFNIÑ</t>
+  </si>
+  <si>
+    <t>SɒFəNZ</t>
+  </si>
+  <si>
+    <t>SɒFTəST</t>
+  </si>
+  <si>
+    <t>SɒFTLÝ/SɒFLÝ</t>
+  </si>
+  <si>
+    <t>SɒFTNəS/SɒFNəS</t>
+  </si>
+  <si>
+    <t>SɒFTSPÖKəN/SɒFSPÖKəN</t>
+  </si>
+  <si>
+    <t>SɒFTWɛR/SɒFWɛR</t>
+  </si>
+  <si>
+    <t>SɒFTWɛRZ/SɒFWɛRZ</t>
+  </si>
+  <si>
+    <t>SɒFTWUD</t>
+  </si>
+  <si>
+    <t>SɒLəMLÝ</t>
+  </si>
+  <si>
+    <t>SɒLSTIS</t>
+  </si>
+  <si>
+    <t>SɒLSTISIS</t>
+  </si>
+  <si>
+    <t>SɒLVəNSÝ</t>
+  </si>
+  <si>
+    <t>SɒLVəNTS</t>
+  </si>
+  <si>
+    <t>SɒÑ</t>
+  </si>
+  <si>
+    <t>SɒÑZ</t>
+  </si>
+  <si>
+    <t>SɒÑB®D</t>
+  </si>
+  <si>
+    <t>SɒÑB®DZ</t>
+  </si>
+  <si>
+    <t>SɒÑ©</t>
+  </si>
+  <si>
+    <t>SɒÑRÍT©</t>
+  </si>
+  <si>
+    <t>SɒÑRÍT©Z</t>
+  </si>
+  <si>
+    <t>SɒÑRÍTIÑ</t>
+  </si>
+  <si>
+    <t>SɒFMɒR</t>
+  </si>
+  <si>
+    <t>SɒFMɒRZ</t>
+  </si>
+  <si>
+    <t>SɒT</t>
+  </si>
+  <si>
+    <t>SPÆZMɒDIK</t>
+  </si>
+  <si>
+    <t>SPÆZMɒDIKLÝ</t>
+  </si>
+  <si>
+    <t>STÆNDɒF</t>
+  </si>
+  <si>
+    <t>STÆNDɒFS</t>
+  </si>
+  <si>
+    <t>STRɛPTəKɒKəS</t>
+  </si>
+  <si>
+    <t>STRɒÑ</t>
+  </si>
+  <si>
+    <t>STRɒÑG©</t>
+  </si>
+  <si>
+    <t>STRɒÑGəST</t>
+  </si>
+  <si>
+    <t>STRɒÑXÖLD</t>
+  </si>
+  <si>
+    <t>STRɒÑXÖLDZ</t>
+  </si>
+  <si>
+    <t>STRɒÑLÝ</t>
+  </si>
+  <si>
+    <t>SWɒMPђ</t>
+  </si>
+  <si>
+    <t>SWɒN©</t>
+  </si>
+  <si>
+    <t>SINəGɒG</t>
+  </si>
+  <si>
+    <t>SINəGɒGZ</t>
+  </si>
+  <si>
+    <t>TÉBəLKLɒθ</t>
+  </si>
+  <si>
+    <t>TÉBəLKLɒθS</t>
+  </si>
+  <si>
+    <t>TÉKɒF</t>
+  </si>
+  <si>
+    <t>TÉKɒFS</t>
+  </si>
+  <si>
+    <t>TÏLÝəLɒJIKəL</t>
+  </si>
+  <si>
+    <t>TÚTɒNIK</t>
+  </si>
+  <si>
+    <t>ÐɛRɒN</t>
+  </si>
+  <si>
+    <t>θɒÑ</t>
+  </si>
+  <si>
+    <t>θÁZəNDYIRZLɒÑ</t>
+  </si>
+  <si>
+    <t>θRɒÑ</t>
+  </si>
+  <si>
+    <t>θRɒÑћ</t>
+  </si>
+  <si>
+    <t>θRɒÑZ</t>
+  </si>
+  <si>
+    <t>TɒF</t>
+  </si>
+  <si>
+    <t>TɒL©ÉTS</t>
+  </si>
+  <si>
+    <t>TɒÑ</t>
+  </si>
+  <si>
+    <t>TɒPDÁN</t>
+  </si>
+  <si>
+    <t>TɒPSÏKRIT</t>
+  </si>
+  <si>
+    <t>TəPɒLəJÝ</t>
+  </si>
+  <si>
+    <t>TɒS</t>
+  </si>
+  <si>
+    <t>TɒSђ</t>
+  </si>
+  <si>
+    <t>TɒSIZ</t>
+  </si>
+  <si>
+    <t>TɒSIÑ</t>
+  </si>
+  <si>
+    <t>TRÉDɒF</t>
+  </si>
+  <si>
+    <t>TRÉDɒFS</t>
+  </si>
+  <si>
+    <t>TRÆVəLɒG</t>
+  </si>
+  <si>
+    <t>TRÏTɒP</t>
+  </si>
+  <si>
+    <t>TRÏTɒPS</t>
+  </si>
+  <si>
+    <t>ʌNKɒNTRəDIKTʔћ</t>
+  </si>
+  <si>
+    <t>ʌND©DɒG</t>
+  </si>
+  <si>
+    <t>ʌND©DɒGZ</t>
+  </si>
+  <si>
+    <t>ʌND©GɒN</t>
+  </si>
+  <si>
+    <t>əNGɒDLÝ</t>
+  </si>
+  <si>
+    <t>əNINVɒLVћ</t>
+  </si>
+  <si>
+    <t>əNWɒNTʔћ</t>
+  </si>
+  <si>
+    <t>VɒLəNTIRIÑ</t>
+  </si>
+  <si>
+    <t>VɒLəNTIRIZəM</t>
+  </si>
+  <si>
+    <t>VUTɒN</t>
+  </si>
+  <si>
+    <t>WɒLəT</t>
+  </si>
+  <si>
+    <t>WɒLəTS</t>
+  </si>
+  <si>
+    <t>WɒLəPIÑ</t>
+  </si>
+  <si>
+    <t>WɒNTʔћ</t>
+  </si>
+  <si>
+    <t>WɔRLɒK</t>
+  </si>
+  <si>
+    <t>WɔRLɒKS</t>
+  </si>
+  <si>
+    <t>WɒʃKLɒθ</t>
+  </si>
+  <si>
+    <t>WɒÇDɒG</t>
+  </si>
+  <si>
+    <t>WɒÇDɒGZ</t>
+  </si>
+  <si>
+    <t>WɔT©BɒTəL</t>
+  </si>
+  <si>
+    <t>WɔT©BɒTəLZ</t>
+  </si>
+  <si>
+    <t>WÖBIGɒN</t>
+  </si>
+  <si>
+    <t>WULFDɒG</t>
+  </si>
+  <si>
+    <t>RÍTɒF</t>
+  </si>
+  <si>
+    <t>RÍTɒFS</t>
+  </si>
+  <si>
+    <t>RɒÑDÚ©</t>
+  </si>
+  <si>
+    <t>RɒÑDÚ©Z</t>
+  </si>
+  <si>
+    <t>RɒÑDÚIÑ</t>
+  </si>
+  <si>
+    <t>RɒÑDÚIÑZ</t>
+  </si>
+  <si>
+    <t>RɒÑћ</t>
+  </si>
+  <si>
+    <t>RɒÑFəL</t>
+  </si>
+  <si>
+    <t>RɒÑFəLÝ</t>
+  </si>
+  <si>
+    <t>RɒÑXɛDʔћ</t>
+  </si>
+  <si>
+    <t>RɒÑLÝ</t>
+  </si>
+  <si>
+    <t>RɒÑZ</t>
+  </si>
+  <si>
+    <t>YIRLɒÑ</t>
   </si>
 </sst>
 </file>
@@ -9531,8 +9912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F877"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A667" workbookViewId="0">
-      <selection activeCell="C682" sqref="C682"/>
+    <sheetView tabSelected="1" topLeftCell="A703" workbookViewId="0">
+      <selection activeCell="C712" sqref="C712"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19099,7 +19480,7 @@
         <v>1008</v>
       </c>
       <c r="C684" t="s">
-        <v>2367</v>
+        <v>3034</v>
       </c>
       <c r="F684" t="s">
         <v>2367</v>
@@ -19127,7 +19508,7 @@
         <v>1385</v>
       </c>
       <c r="C686" t="s">
-        <v>2369</v>
+        <v>3035</v>
       </c>
       <c r="F686" t="s">
         <v>2369</v>
@@ -19141,7 +19522,7 @@
         <v>1386</v>
       </c>
       <c r="C687" t="s">
-        <v>2370</v>
+        <v>3036</v>
       </c>
       <c r="F687" t="s">
         <v>2370</v>
@@ -19155,7 +19536,7 @@
         <v>1395</v>
       </c>
       <c r="C688" t="s">
-        <v>2371</v>
+        <v>3037</v>
       </c>
       <c r="F688" t="s">
         <v>2371</v>
@@ -19169,7 +19550,7 @@
         <v>1012</v>
       </c>
       <c r="C689" t="s">
-        <v>2372</v>
+        <v>3038</v>
       </c>
       <c r="F689" t="s">
         <v>2372</v>
@@ -19183,7 +19564,7 @@
         <v>1384</v>
       </c>
       <c r="C690" t="s">
-        <v>2373</v>
+        <v>3039</v>
       </c>
       <c r="F690" t="s">
         <v>2373</v>
@@ -19197,7 +19578,7 @@
         <v>1396</v>
       </c>
       <c r="C691" t="s">
-        <v>2374</v>
+        <v>3040</v>
       </c>
       <c r="F691" t="s">
         <v>2374</v>
@@ -19211,7 +19592,7 @@
         <v>1035</v>
       </c>
       <c r="C692" t="s">
-        <v>2375</v>
+        <v>3041</v>
       </c>
       <c r="F692" t="s">
         <v>2375</v>
@@ -19225,7 +19606,7 @@
         <v>1041</v>
       </c>
       <c r="C693" t="s">
-        <v>2376</v>
+        <v>3042</v>
       </c>
       <c r="F693" t="s">
         <v>2376</v>
@@ -19239,7 +19620,7 @@
         <v>1044</v>
       </c>
       <c r="C694" t="s">
-        <v>2377</v>
+        <v>3043</v>
       </c>
       <c r="F694" t="s">
         <v>2377</v>
@@ -19253,7 +19634,7 @@
         <v>1045</v>
       </c>
       <c r="C695" t="s">
-        <v>2378</v>
+        <v>3044</v>
       </c>
       <c r="F695" t="s">
         <v>2378</v>
@@ -19295,7 +19676,7 @@
         <v>1019</v>
       </c>
       <c r="C698" t="s">
-        <v>2381</v>
+        <v>3045</v>
       </c>
       <c r="F698" t="s">
         <v>2381</v>
@@ -19309,7 +19690,7 @@
         <v>1021</v>
       </c>
       <c r="C699" t="s">
-        <v>2382</v>
+        <v>3046</v>
       </c>
       <c r="F699" t="s">
         <v>2382</v>
@@ -19323,7 +19704,7 @@
         <v>1020</v>
       </c>
       <c r="C700" t="s">
-        <v>2383</v>
+        <v>3047</v>
       </c>
       <c r="F700" t="s">
         <v>2383</v>
@@ -19365,7 +19746,7 @@
         <v>1022</v>
       </c>
       <c r="C703" t="s">
-        <v>2386</v>
+        <v>3048</v>
       </c>
       <c r="F703" t="s">
         <v>2386</v>
@@ -19379,7 +19760,7 @@
         <v>1023</v>
       </c>
       <c r="C704" t="s">
-        <v>2387</v>
+        <v>3049</v>
       </c>
       <c r="F704" t="s">
         <v>2387</v>
@@ -19393,7 +19774,7 @@
         <v>1024</v>
       </c>
       <c r="C705" t="s">
-        <v>2388</v>
+        <v>3050</v>
       </c>
       <c r="F705" t="s">
         <v>2388</v>
@@ -19407,7 +19788,7 @@
         <v>1400</v>
       </c>
       <c r="C706" t="s">
-        <v>2389</v>
+        <v>3051</v>
       </c>
       <c r="F706" t="s">
         <v>2389</v>
@@ -19421,7 +19802,7 @@
         <v>1410</v>
       </c>
       <c r="C707" t="s">
-        <v>2390</v>
+        <v>3052</v>
       </c>
       <c r="F707" t="s">
         <v>2390</v>
@@ -19435,7 +19816,7 @@
         <v>1428</v>
       </c>
       <c r="C708" t="s">
-        <v>2391</v>
+        <v>3053</v>
       </c>
       <c r="F708" t="s">
         <v>2391</v>
@@ -19463,7 +19844,7 @@
         <v>1423</v>
       </c>
       <c r="C710" t="s">
-        <v>2393</v>
+        <v>3054</v>
       </c>
       <c r="F710" t="s">
         <v>2393</v>
@@ -19477,7 +19858,7 @@
         <v>1424</v>
       </c>
       <c r="C711" t="s">
-        <v>2394</v>
+        <v>3055</v>
       </c>
       <c r="F711" t="s">
         <v>2394</v>
@@ -19505,7 +19886,7 @@
         <v>1412</v>
       </c>
       <c r="C713" t="s">
-        <v>2396</v>
+        <v>3056</v>
       </c>
       <c r="F713" t="s">
         <v>2396</v>
@@ -19519,7 +19900,7 @@
         <v>1414</v>
       </c>
       <c r="C714" t="s">
-        <v>2397</v>
+        <v>3057</v>
       </c>
       <c r="F714" t="s">
         <v>2397</v>
@@ -19533,7 +19914,7 @@
         <v>1415</v>
       </c>
       <c r="C715" t="s">
-        <v>2398</v>
+        <v>3058</v>
       </c>
       <c r="F715" t="s">
         <v>2398</v>
@@ -19547,7 +19928,7 @@
         <v>1413</v>
       </c>
       <c r="C716" t="s">
-        <v>2399</v>
+        <v>3059</v>
       </c>
       <c r="F716" t="s">
         <v>2399</v>
@@ -19575,7 +19956,7 @@
         <v>1422</v>
       </c>
       <c r="C718" t="s">
-        <v>2401</v>
+        <v>3060</v>
       </c>
       <c r="F718" t="s">
         <v>2401</v>
@@ -19589,7 +19970,7 @@
         <v>1416</v>
       </c>
       <c r="C719" t="s">
-        <v>2402</v>
+        <v>3061</v>
       </c>
       <c r="F719" t="s">
         <v>2402</v>
@@ -19603,7 +19984,7 @@
         <v>1417</v>
       </c>
       <c r="C720" t="s">
-        <v>2403</v>
+        <v>3062</v>
       </c>
       <c r="F720" t="s">
         <v>2403</v>
@@ -19617,7 +19998,7 @@
         <v>1425</v>
       </c>
       <c r="C721" t="s">
-        <v>2404</v>
+        <v>3063</v>
       </c>
       <c r="F721" t="s">
         <v>2404</v>
@@ -19631,7 +20012,7 @@
         <v>1418</v>
       </c>
       <c r="C722" t="s">
-        <v>2405</v>
+        <v>3064</v>
       </c>
       <c r="F722" t="s">
         <v>2405</v>
@@ -19645,7 +20026,7 @@
         <v>1419</v>
       </c>
       <c r="C723" t="s">
-        <v>2406</v>
+        <v>3065</v>
       </c>
       <c r="F723" t="s">
         <v>2406</v>
@@ -19659,7 +20040,7 @@
         <v>1420</v>
       </c>
       <c r="C724" t="s">
-        <v>2407</v>
+        <v>3066</v>
       </c>
       <c r="F724" t="s">
         <v>2407</v>
@@ -19673,7 +20054,7 @@
         <v>1433</v>
       </c>
       <c r="C725" t="s">
-        <v>2408</v>
+        <v>3067</v>
       </c>
       <c r="F725" t="s">
         <v>2408</v>
@@ -19687,7 +20068,7 @@
         <v>1429</v>
       </c>
       <c r="C726" t="s">
-        <v>2409</v>
+        <v>3068</v>
       </c>
       <c r="F726" t="s">
         <v>2409</v>
@@ -19701,7 +20082,7 @@
         <v>1430</v>
       </c>
       <c r="C727" t="s">
-        <v>2410</v>
+        <v>3069</v>
       </c>
       <c r="F727" t="s">
         <v>2410</v>
@@ -19715,7 +20096,7 @@
         <v>1431</v>
       </c>
       <c r="C728" t="s">
-        <v>2411</v>
+        <v>3070</v>
       </c>
       <c r="F728" t="s">
         <v>2411</v>
@@ -19729,7 +20110,7 @@
         <v>1432</v>
       </c>
       <c r="C729" t="s">
-        <v>2412</v>
+        <v>3071</v>
       </c>
       <c r="F729" t="s">
         <v>2412</v>
@@ -19743,7 +20124,7 @@
         <v>1038</v>
       </c>
       <c r="C730" t="s">
-        <v>2413</v>
+        <v>3072</v>
       </c>
       <c r="F730" t="s">
         <v>2413</v>
@@ -19757,7 +20138,7 @@
         <v>1039</v>
       </c>
       <c r="C731" t="s">
-        <v>2414</v>
+        <v>3073</v>
       </c>
       <c r="F731" t="s">
         <v>2414</v>
@@ -19771,7 +20152,7 @@
         <v>1436</v>
       </c>
       <c r="C732" t="s">
-        <v>2415</v>
+        <v>3074</v>
       </c>
       <c r="F732" t="s">
         <v>2415</v>
@@ -19785,7 +20166,7 @@
         <v>1437</v>
       </c>
       <c r="C733" t="s">
-        <v>2416</v>
+        <v>3075</v>
       </c>
       <c r="F733" t="s">
         <v>2416</v>
@@ -19799,7 +20180,7 @@
         <v>1438</v>
       </c>
       <c r="C734" t="s">
-        <v>2417</v>
+        <v>3076</v>
       </c>
       <c r="F734" t="s">
         <v>2417</v>
@@ -19813,7 +20194,7 @@
         <v>1439</v>
       </c>
       <c r="C735" t="s">
-        <v>2418</v>
+        <v>3077</v>
       </c>
       <c r="F735" t="s">
         <v>2418</v>
@@ -19827,7 +20208,7 @@
         <v>1440</v>
       </c>
       <c r="C736" t="s">
-        <v>2419</v>
+        <v>3078</v>
       </c>
       <c r="F736" t="s">
         <v>2419</v>
@@ -19841,7 +20222,7 @@
         <v>1441</v>
       </c>
       <c r="C737" t="s">
-        <v>2420</v>
+        <v>3079</v>
       </c>
       <c r="F737" t="s">
         <v>2420</v>
@@ -19855,7 +20236,7 @@
         <v>1426</v>
       </c>
       <c r="C738" t="s">
-        <v>2421</v>
+        <v>3080</v>
       </c>
       <c r="F738" t="s">
         <v>2421</v>
@@ -19869,7 +20250,7 @@
         <v>1427</v>
       </c>
       <c r="C739" t="s">
-        <v>2422</v>
+        <v>3081</v>
       </c>
       <c r="F739" t="s">
         <v>2422</v>
@@ -19925,7 +20306,7 @@
         <v>1037</v>
       </c>
       <c r="C743" t="s">
-        <v>2426</v>
+        <v>3082</v>
       </c>
       <c r="F743" t="s">
         <v>2426</v>
@@ -19939,7 +20320,7 @@
         <v>1025</v>
       </c>
       <c r="C744" t="s">
-        <v>2427</v>
+        <v>3083</v>
       </c>
       <c r="F744" t="s">
         <v>2427</v>
@@ -19953,7 +20334,7 @@
         <v>1026</v>
       </c>
       <c r="C745" t="s">
-        <v>2428</v>
+        <v>3084</v>
       </c>
       <c r="F745" t="s">
         <v>2428</v>
@@ -19981,7 +20362,7 @@
         <v>1407</v>
       </c>
       <c r="C747" t="s">
-        <v>2430</v>
+        <v>3085</v>
       </c>
       <c r="F747" t="s">
         <v>2430</v>
@@ -19995,7 +20376,7 @@
         <v>1645</v>
       </c>
       <c r="C748" t="s">
-        <v>2431</v>
+        <v>3086</v>
       </c>
       <c r="F748" t="s">
         <v>2431</v>
@@ -20009,7 +20390,7 @@
         <v>1028</v>
       </c>
       <c r="C749" t="s">
-        <v>2432</v>
+        <v>3087</v>
       </c>
       <c r="F749" t="s">
         <v>2432</v>
@@ -20023,7 +20404,7 @@
         <v>1401</v>
       </c>
       <c r="C750" t="s">
-        <v>2433</v>
+        <v>3088</v>
       </c>
       <c r="F750" t="s">
         <v>2433</v>
@@ -20037,7 +20418,7 @@
         <v>1402</v>
       </c>
       <c r="C751" t="s">
-        <v>2434</v>
+        <v>3089</v>
       </c>
       <c r="F751" t="s">
         <v>2434</v>
@@ -20051,7 +20432,7 @@
         <v>1403</v>
       </c>
       <c r="C752" t="s">
-        <v>2435</v>
+        <v>3090</v>
       </c>
       <c r="F752" t="s">
         <v>2435</v>
@@ -20065,7 +20446,7 @@
         <v>1404</v>
       </c>
       <c r="C753" t="s">
-        <v>2436</v>
+        <v>3091</v>
       </c>
       <c r="F753" t="s">
         <v>2436</v>
@@ -20079,7 +20460,7 @@
         <v>1405</v>
       </c>
       <c r="C754" t="s">
-        <v>2437</v>
+        <v>3092</v>
       </c>
       <c r="F754" t="s">
         <v>2437</v>
@@ -20093,7 +20474,7 @@
         <v>1027</v>
       </c>
       <c r="C755" t="s">
-        <v>2438</v>
+        <v>3093</v>
       </c>
       <c r="F755" t="s">
         <v>2438</v>
@@ -20163,7 +20544,7 @@
         <v>1031</v>
       </c>
       <c r="C760" t="s">
-        <v>2443</v>
+        <v>3094</v>
       </c>
       <c r="F760" t="s">
         <v>2443</v>
@@ -20205,7 +20586,7 @@
         <v>1409</v>
       </c>
       <c r="C763" t="s">
-        <v>2446</v>
+        <v>3095</v>
       </c>
       <c r="F763" t="s">
         <v>2446</v>
@@ -20247,7 +20628,7 @@
         <v>1442</v>
       </c>
       <c r="C766" t="s">
-        <v>2449</v>
+        <v>3096</v>
       </c>
       <c r="F766" t="s">
         <v>2449</v>
@@ -20261,7 +20642,7 @@
         <v>1443</v>
       </c>
       <c r="C767" t="s">
-        <v>2450</v>
+        <v>3097</v>
       </c>
       <c r="F767" t="s">
         <v>2450</v>
@@ -20275,7 +20656,7 @@
         <v>1444</v>
       </c>
       <c r="C768" t="s">
-        <v>2451</v>
+        <v>3098</v>
       </c>
       <c r="F768" t="s">
         <v>2451</v>
@@ -20289,7 +20670,7 @@
         <v>1445</v>
       </c>
       <c r="C769" t="s">
-        <v>2452</v>
+        <v>3099</v>
       </c>
       <c r="F769" t="s">
         <v>2452</v>
@@ -20303,7 +20684,7 @@
         <v>1446</v>
       </c>
       <c r="C770" t="s">
-        <v>2453</v>
+        <v>3100</v>
       </c>
       <c r="F770" t="s">
         <v>2453</v>
@@ -20317,7 +20698,7 @@
         <v>1447</v>
       </c>
       <c r="C771" t="s">
-        <v>2454</v>
+        <v>3101</v>
       </c>
       <c r="F771" t="s">
         <v>2454</v>
@@ -20331,7 +20712,7 @@
         <v>1063</v>
       </c>
       <c r="C772" t="s">
-        <v>2455</v>
+        <v>3102</v>
       </c>
       <c r="F772" t="s">
         <v>2455</v>
@@ -20345,7 +20726,7 @@
         <v>1046</v>
       </c>
       <c r="C773" t="s">
-        <v>2456</v>
+        <v>3103</v>
       </c>
       <c r="F773" t="s">
         <v>2456</v>
@@ -20359,7 +20740,7 @@
         <v>1079</v>
       </c>
       <c r="C774" t="s">
-        <v>2457</v>
+        <v>3104</v>
       </c>
       <c r="F774" t="s">
         <v>2457</v>
@@ -20373,7 +20754,7 @@
         <v>1684</v>
       </c>
       <c r="C775" t="s">
-        <v>2458</v>
+        <v>3105</v>
       </c>
       <c r="F775" t="s">
         <v>2458</v>
@@ -20387,7 +20768,7 @@
         <v>1589</v>
       </c>
       <c r="C776" t="s">
-        <v>2459</v>
+        <v>3106</v>
       </c>
       <c r="F776" t="s">
         <v>2459</v>
@@ -20401,7 +20782,7 @@
         <v>1681</v>
       </c>
       <c r="C777" t="s">
-        <v>2460</v>
+        <v>3107</v>
       </c>
       <c r="F777" t="s">
         <v>2460</v>
@@ -20415,7 +20796,7 @@
         <v>1682</v>
       </c>
       <c r="C778" t="s">
-        <v>2461</v>
+        <v>3108</v>
       </c>
       <c r="F778" t="s">
         <v>2461</v>
@@ -20429,7 +20810,7 @@
         <v>1683</v>
       </c>
       <c r="C779" t="s">
-        <v>2462</v>
+        <v>3109</v>
       </c>
       <c r="F779" t="s">
         <v>2462</v>
@@ -20443,7 +20824,7 @@
         <v>1051</v>
       </c>
       <c r="C780" t="s">
-        <v>2463</v>
+        <v>3110</v>
       </c>
       <c r="F780" t="s">
         <v>2463</v>
@@ -20457,7 +20838,7 @@
         <v>1451</v>
       </c>
       <c r="C781" t="s">
-        <v>2464</v>
+        <v>3111</v>
       </c>
       <c r="F781" t="s">
         <v>2464</v>
@@ -20499,7 +20880,7 @@
         <v>1057</v>
       </c>
       <c r="C784" t="s">
-        <v>2467</v>
+        <v>3112</v>
       </c>
       <c r="F784" t="s">
         <v>2467</v>
@@ -20541,7 +20922,7 @@
         <v>1053</v>
       </c>
       <c r="C787" t="s">
-        <v>2470</v>
+        <v>3113</v>
       </c>
       <c r="F787" t="s">
         <v>2470</v>
@@ -20555,7 +20936,7 @@
         <v>1054</v>
       </c>
       <c r="C788" t="s">
-        <v>2471</v>
+        <v>3114</v>
       </c>
       <c r="F788" t="s">
         <v>2471</v>
@@ -20569,7 +20950,7 @@
         <v>1060</v>
       </c>
       <c r="C789" t="s">
-        <v>2472</v>
+        <v>3115</v>
       </c>
       <c r="F789" t="s">
         <v>2472</v>
@@ -20667,7 +21048,7 @@
         <v>1055</v>
       </c>
       <c r="C796" t="s">
-        <v>2479</v>
+        <v>3116</v>
       </c>
       <c r="F796" t="s">
         <v>2479</v>
@@ -20681,7 +21062,7 @@
         <v>1056</v>
       </c>
       <c r="C797" t="s">
-        <v>2480</v>
+        <v>3117</v>
       </c>
       <c r="F797" t="s">
         <v>2480</v>
@@ -20695,7 +21076,7 @@
         <v>1457</v>
       </c>
       <c r="C798" t="s">
-        <v>2481</v>
+        <v>3118</v>
       </c>
       <c r="F798" t="s">
         <v>2481</v>
@@ -20709,7 +21090,7 @@
         <v>1458</v>
       </c>
       <c r="C799" t="s">
-        <v>2482</v>
+        <v>3119</v>
       </c>
       <c r="F799" t="s">
         <v>2482</v>
@@ -20723,7 +21104,7 @@
         <v>1047</v>
       </c>
       <c r="C800" t="s">
-        <v>2483</v>
+        <v>3120</v>
       </c>
       <c r="F800" t="s">
         <v>2483</v>
@@ -20737,7 +21118,7 @@
         <v>1048</v>
       </c>
       <c r="C801" t="s">
-        <v>2484</v>
+        <v>3121</v>
       </c>
       <c r="F801" t="s">
         <v>2484</v>
@@ -20751,7 +21132,7 @@
         <v>1450</v>
       </c>
       <c r="C802" t="s">
-        <v>2485</v>
+        <v>3122</v>
       </c>
       <c r="F802" t="s">
         <v>2485</v>
@@ -20765,7 +21146,7 @@
         <v>1448</v>
       </c>
       <c r="C803" t="s">
-        <v>2486</v>
+        <v>3123</v>
       </c>
       <c r="F803" t="s">
         <v>2486</v>
@@ -20779,7 +21160,7 @@
         <v>1449</v>
       </c>
       <c r="C804" t="s">
-        <v>2487</v>
+        <v>3124</v>
       </c>
       <c r="F804" t="s">
         <v>2487</v>
@@ -20821,7 +21202,7 @@
         <v>1680</v>
       </c>
       <c r="C807" t="s">
-        <v>2490</v>
+        <v>3125</v>
       </c>
       <c r="F807" t="s">
         <v>2490</v>
@@ -20835,7 +21216,7 @@
         <v>1582</v>
       </c>
       <c r="C808" t="s">
-        <v>2491</v>
+        <v>3126</v>
       </c>
       <c r="F808" t="s">
         <v>2491</v>
@@ -20849,7 +21230,7 @@
         <v>1583</v>
       </c>
       <c r="C809" t="s">
-        <v>2492</v>
+        <v>3127</v>
       </c>
       <c r="F809" t="s">
         <v>2492</v>
@@ -20863,7 +21244,7 @@
         <v>1674</v>
       </c>
       <c r="C810" t="s">
-        <v>2493</v>
+        <v>3128</v>
       </c>
       <c r="F810" t="s">
         <v>2493</v>
@@ -20877,7 +21258,7 @@
         <v>1134</v>
       </c>
       <c r="C811" t="s">
-        <v>2494</v>
+        <v>3129</v>
       </c>
       <c r="F811" t="s">
         <v>2494</v>
@@ -20905,7 +21286,7 @@
         <v>1676</v>
       </c>
       <c r="C813" t="s">
-        <v>2496</v>
+        <v>3130</v>
       </c>
       <c r="F813" t="s">
         <v>2496</v>
@@ -20975,7 +21356,7 @@
         <v>1136</v>
       </c>
       <c r="C818" t="s">
-        <v>2501</v>
+        <v>3131</v>
       </c>
       <c r="F818" t="s">
         <v>2501</v>
@@ -21031,7 +21412,7 @@
         <v>1648</v>
       </c>
       <c r="C822" t="s">
-        <v>2505</v>
+        <v>3132</v>
       </c>
       <c r="F822" t="s">
         <v>2505</v>
@@ -21045,7 +21426,7 @@
         <v>1647</v>
       </c>
       <c r="C823" t="s">
-        <v>2506</v>
+        <v>3133</v>
       </c>
       <c r="F823" t="s">
         <v>2506</v>
@@ -21073,7 +21454,7 @@
         <v>1064</v>
       </c>
       <c r="C825" t="s">
-        <v>2508</v>
+        <v>3134</v>
       </c>
       <c r="F825" t="s">
         <v>2508</v>
@@ -21129,7 +21510,7 @@
         <v>1464</v>
       </c>
       <c r="C829" t="s">
-        <v>2512</v>
+        <v>3135</v>
       </c>
       <c r="F829" t="s">
         <v>2512</v>
@@ -21143,7 +21524,7 @@
         <v>1465</v>
       </c>
       <c r="C830" t="s">
-        <v>2513</v>
+        <v>3136</v>
       </c>
       <c r="F830" t="s">
         <v>2513</v>
@@ -21157,7 +21538,7 @@
         <v>1461</v>
       </c>
       <c r="C831" t="s">
-        <v>2514</v>
+        <v>3137</v>
       </c>
       <c r="F831" t="s">
         <v>2514</v>
@@ -21185,7 +21566,7 @@
         <v>1468</v>
       </c>
       <c r="C833" t="s">
-        <v>2516</v>
+        <v>3138</v>
       </c>
       <c r="F833" t="s">
         <v>2516</v>
@@ -21241,7 +21622,7 @@
         <v>1487</v>
       </c>
       <c r="C837" t="s">
-        <v>2520</v>
+        <v>3139</v>
       </c>
       <c r="F837" t="s">
         <v>2520</v>
@@ -21255,7 +21636,7 @@
         <v>1488</v>
       </c>
       <c r="C838" t="s">
-        <v>2521</v>
+        <v>3140</v>
       </c>
       <c r="F838" t="s">
         <v>2521</v>
@@ -21451,7 +21832,7 @@
         <v>1482</v>
       </c>
       <c r="C852" t="s">
-        <v>2535</v>
+        <v>3141</v>
       </c>
       <c r="F852" t="s">
         <v>2535</v>
@@ -21507,7 +21888,7 @@
         <v>1485</v>
       </c>
       <c r="C856" t="s">
-        <v>2539</v>
+        <v>3142</v>
       </c>
       <c r="F856" t="s">
         <v>2539</v>
@@ -21521,7 +21902,7 @@
         <v>1486</v>
       </c>
       <c r="C857" t="s">
-        <v>2540</v>
+        <v>3143</v>
       </c>
       <c r="F857" t="s">
         <v>2540</v>
@@ -21549,7 +21930,7 @@
         <v>1491</v>
       </c>
       <c r="C859" t="s">
-        <v>2542</v>
+        <v>3144</v>
       </c>
       <c r="F859" t="s">
         <v>2542</v>
@@ -21563,7 +21944,7 @@
         <v>1492</v>
       </c>
       <c r="C860" t="s">
-        <v>2543</v>
+        <v>3145</v>
       </c>
       <c r="F860" t="s">
         <v>2543</v>
@@ -21605,7 +21986,7 @@
         <v>1493</v>
       </c>
       <c r="C863" t="s">
-        <v>2546</v>
+        <v>3146</v>
       </c>
       <c r="F863" t="s">
         <v>2546</v>
@@ -21619,7 +22000,7 @@
         <v>1071</v>
       </c>
       <c r="C864" t="s">
-        <v>2547</v>
+        <v>3147</v>
       </c>
       <c r="F864" t="s">
         <v>2547</v>
@@ -21633,7 +22014,7 @@
         <v>1380</v>
       </c>
       <c r="C865" t="s">
-        <v>2548</v>
+        <v>3148</v>
       </c>
       <c r="F865" t="s">
         <v>2548</v>
@@ -21647,7 +22028,7 @@
         <v>1381</v>
       </c>
       <c r="C866" t="s">
-        <v>2549</v>
+        <v>3149</v>
       </c>
       <c r="F866" t="s">
         <v>2549</v>
@@ -21661,7 +22042,7 @@
         <v>1392</v>
       </c>
       <c r="C867" t="s">
-        <v>2550</v>
+        <v>3150</v>
       </c>
       <c r="F867" t="s">
         <v>2550</v>
@@ -21675,7 +22056,7 @@
         <v>1393</v>
       </c>
       <c r="C868" t="s">
-        <v>2551</v>
+        <v>3151</v>
       </c>
       <c r="F868" t="s">
         <v>2551</v>
@@ -21689,7 +22070,7 @@
         <v>1390</v>
       </c>
       <c r="C869" t="s">
-        <v>2552</v>
+        <v>3152</v>
       </c>
       <c r="F869" t="s">
         <v>2552</v>
@@ -21703,7 +22084,7 @@
         <v>1391</v>
       </c>
       <c r="C870" t="s">
-        <v>2553</v>
+        <v>3153</v>
       </c>
       <c r="F870" t="s">
         <v>2553</v>
@@ -21717,7 +22098,7 @@
         <v>1010</v>
       </c>
       <c r="C871" t="s">
-        <v>2554</v>
+        <v>3154</v>
       </c>
       <c r="F871" t="s">
         <v>2554</v>
@@ -21731,7 +22112,7 @@
         <v>1387</v>
       </c>
       <c r="C872" t="s">
-        <v>2555</v>
+        <v>3155</v>
       </c>
       <c r="F872" t="s">
         <v>2555</v>
@@ -21745,7 +22126,7 @@
         <v>1388</v>
       </c>
       <c r="C873" t="s">
-        <v>2556</v>
+        <v>3156</v>
       </c>
       <c r="F873" t="s">
         <v>2556</v>
@@ -21759,7 +22140,7 @@
         <v>1394</v>
       </c>
       <c r="C874" t="s">
-        <v>2557</v>
+        <v>3157</v>
       </c>
       <c r="F874" t="s">
         <v>2557</v>
@@ -21773,7 +22154,7 @@
         <v>1389</v>
       </c>
       <c r="C875" t="s">
-        <v>2558</v>
+        <v>3158</v>
       </c>
       <c r="F875" t="s">
         <v>2558</v>
@@ -21787,7 +22168,7 @@
         <v>1011</v>
       </c>
       <c r="C876" t="s">
-        <v>2559</v>
+        <v>3159</v>
       </c>
       <c r="F876" t="s">
         <v>2559</v>
@@ -21801,7 +22182,7 @@
         <v>1171</v>
       </c>
       <c r="C877" t="s">
-        <v>2560</v>
+        <v>3160</v>
       </c>
       <c r="F877" t="s">
         <v>2560</v>

</xml_diff>